<commit_message>
adding PCA part in 3
</commit_message>
<xml_diff>
--- a/out/diabetes_join.xlsx
+++ b/out/diabetes_join.xlsx
@@ -860,7 +860,7 @@
       </c>
       <c r="K11" t="inlineStr">
         <is>
-          <t>P%rivate</t>
+          <t>Private</t>
         </is>
       </c>
     </row>
@@ -1760,7 +1760,7 @@
       </c>
       <c r="K31" t="inlineStr">
         <is>
-          <t>Priva.te</t>
+          <t>Private</t>
         </is>
       </c>
     </row>
@@ -1805,7 +1805,7 @@
       </c>
       <c r="K32" t="inlineStr">
         <is>
-          <t>Self-employe)d</t>
+          <t>Self-employed</t>
         </is>
       </c>
     </row>
@@ -2235,7 +2235,7 @@
       </c>
       <c r="K42" t="inlineStr">
         <is>
-          <t>*Public</t>
+          <t>Public</t>
         </is>
       </c>
     </row>
@@ -2730,7 +2730,7 @@
       </c>
       <c r="K53" t="inlineStr">
         <is>
-          <t>Pu.blic</t>
+          <t>Public</t>
         </is>
       </c>
     </row>
@@ -2910,7 +2910,7 @@
       </c>
       <c r="K57" t="inlineStr">
         <is>
-          <t>S@elf-employed</t>
+          <t>Self-employed</t>
         </is>
       </c>
     </row>
@@ -3315,7 +3315,7 @@
       </c>
       <c r="K66" t="inlineStr">
         <is>
-          <t>Publi-c</t>
+          <t>Public</t>
         </is>
       </c>
     </row>
@@ -6820,11 +6820,6 @@
           <t>Yes</t>
         </is>
       </c>
-      <c r="K144" t="inlineStr">
-        <is>
-          <t>Retired</t>
-        </is>
-      </c>
     </row>
     <row r="145">
       <c r="A145">
@@ -6997,7 +6992,7 @@
       </c>
       <c r="K148" t="inlineStr">
         <is>
-          <t>Publ&amp;ic</t>
+          <t>Public</t>
         </is>
       </c>
     </row>
@@ -7447,7 +7442,7 @@
       </c>
       <c r="K158" t="inlineStr">
         <is>
-          <t>Self-emplo$yed</t>
+          <t>Self-employed</t>
         </is>
       </c>
     </row>
@@ -7985,11 +7980,6 @@
           <t>Yes</t>
         </is>
       </c>
-      <c r="K170" t="inlineStr">
-        <is>
-          <t>Retired</t>
-        </is>
-      </c>
     </row>
     <row r="171">
       <c r="A171">
@@ -8662,7 +8652,7 @@
       </c>
       <c r="K185" t="inlineStr">
         <is>
-          <t>P!UBLIC</t>
+          <t>Public</t>
         </is>
       </c>
     </row>
@@ -8932,7 +8922,7 @@
       </c>
       <c r="K191" t="inlineStr">
         <is>
-          <t>Privat+e</t>
+          <t>Private</t>
         </is>
       </c>
     </row>
@@ -9382,7 +9372,7 @@
       </c>
       <c r="K201" t="inlineStr">
         <is>
-          <t>SELF-EMPLOYED</t>
+          <t>Self-employed</t>
         </is>
       </c>
     </row>
@@ -9470,11 +9460,6 @@
           <t>No</t>
         </is>
       </c>
-      <c r="K203" t="inlineStr">
-        <is>
-          <t>P-ublic</t>
-        </is>
-      </c>
     </row>
     <row r="204">
       <c r="A204">
@@ -11180,11 +11165,6 @@
           <t>No</t>
         </is>
       </c>
-      <c r="K241" t="inlineStr">
-        <is>
-          <t>Retired</t>
-        </is>
-      </c>
     </row>
     <row r="242">
       <c r="A242">
@@ -11805,11 +11785,6 @@
           <t>0</t>
         </is>
       </c>
-      <c r="K255" t="inlineStr">
-        <is>
-          <t>Retired</t>
-        </is>
-      </c>
     </row>
     <row r="256">
       <c r="A256">
@@ -12527,7 +12502,7 @@
       </c>
       <c r="K271" t="inlineStr">
         <is>
-          <t>Se.lf-employed</t>
+          <t>Self-employed</t>
         </is>
       </c>
     </row>
@@ -15249,7 +15224,7 @@
       </c>
       <c r="K332" t="inlineStr">
         <is>
-          <t>-Public</t>
+          <t>Public</t>
         </is>
       </c>
     </row>
@@ -15339,7 +15314,7 @@
       </c>
       <c r="K334" t="inlineStr">
         <is>
-          <t>Publi+c</t>
+          <t>Public</t>
         </is>
       </c>
     </row>
@@ -17679,7 +17654,7 @@
       </c>
       <c r="K386" t="inlineStr">
         <is>
-          <t>Self.-employed</t>
+          <t>Self-employed</t>
         </is>
       </c>
     </row>
@@ -21606,7 +21581,7 @@
       </c>
       <c r="K474" t="inlineStr">
         <is>
-          <t>Privat-e</t>
+          <t>Private</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
adding whitespace and str_trim
</commit_message>
<xml_diff>
--- a/out/diabetes_join.xlsx
+++ b/out/diabetes_join.xlsx
@@ -2113,6 +2113,16 @@
           <t>1</t>
         </is>
       </c>
+      <c r="J39" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="K39" t="inlineStr">
+        <is>
+          <t>Public</t>
+        </is>
+      </c>
     </row>
     <row r="40">
       <c r="A40">
@@ -2193,6 +2203,16 @@
           <t>0</t>
         </is>
       </c>
+      <c r="J41" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="K41" t="inlineStr">
+        <is>
+          <t>Public</t>
+        </is>
+      </c>
     </row>
     <row r="42">
       <c r="A42">
@@ -6820,6 +6840,11 @@
           <t>Yes</t>
         </is>
       </c>
+      <c r="K144" t="inlineStr">
+        <is>
+          <t>Retired</t>
+        </is>
+      </c>
     </row>
     <row r="145">
       <c r="A145">
@@ -6945,6 +6970,11 @@
           <t>0</t>
         </is>
       </c>
+      <c r="J147" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
       <c r="K147" t="inlineStr">
         <is>
           <t>Private</t>
@@ -7980,6 +8010,11 @@
           <t>Yes</t>
         </is>
       </c>
+      <c r="K170" t="inlineStr">
+        <is>
+          <t>Retired</t>
+        </is>
+      </c>
     </row>
     <row r="171">
       <c r="A171">
@@ -9460,6 +9495,11 @@
           <t>No</t>
         </is>
       </c>
+      <c r="K203" t="inlineStr">
+        <is>
+          <t>Public</t>
+        </is>
+      </c>
     </row>
     <row r="204">
       <c r="A204">
@@ -11165,6 +11205,11 @@
           <t>No</t>
         </is>
       </c>
+      <c r="K241" t="inlineStr">
+        <is>
+          <t>Retired</t>
+        </is>
+      </c>
     </row>
     <row r="242">
       <c r="A242">
@@ -11785,6 +11830,16 @@
           <t>0</t>
         </is>
       </c>
+      <c r="J255" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="K255" t="inlineStr">
+        <is>
+          <t>Retired</t>
+        </is>
+      </c>
     </row>
     <row r="256">
       <c r="A256">
@@ -12720,6 +12775,16 @@
           <t>1</t>
         </is>
       </c>
+      <c r="J276" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="K276" t="inlineStr">
+        <is>
+          <t>Private</t>
+        </is>
+      </c>
     </row>
     <row r="277">
       <c r="A277">
@@ -14417,6 +14482,16 @@
           <t>0</t>
         </is>
       </c>
+      <c r="J314" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="K314" t="inlineStr">
+        <is>
+          <t>Public</t>
+        </is>
+      </c>
     </row>
     <row r="315">
       <c r="A315">
@@ -18142,6 +18217,11 @@
           <t>0</t>
         </is>
       </c>
+      <c r="J397" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
       <c r="K397" t="inlineStr">
         <is>
           <t>Public</t>
@@ -19799,6 +19879,11 @@
           <t>1</t>
         </is>
       </c>
+      <c r="J434" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
       <c r="K434" t="inlineStr">
         <is>
           <t>Public</t>
@@ -19884,6 +19969,16 @@
           <t>1</t>
         </is>
       </c>
+      <c r="J436" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="K436" t="inlineStr">
+        <is>
+          <t>Private</t>
+        </is>
+      </c>
     </row>
     <row r="437">
       <c r="A437">
@@ -20009,6 +20104,11 @@
           <t>1</t>
         </is>
       </c>
+      <c r="J439" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
       <c r="K439" t="inlineStr">
         <is>
           <t>Self-employed</t>
@@ -20999,6 +21099,11 @@
           <t>No</t>
         </is>
       </c>
+      <c r="K461" t="inlineStr">
+        <is>
+          <t>Private</t>
+        </is>
+      </c>
     </row>
     <row r="462">
       <c r="A462">
@@ -21667,6 +21772,11 @@
       <c r="J476" t="inlineStr">
         <is>
           <t>No</t>
+        </is>
+      </c>
+      <c r="K476" t="inlineStr">
+        <is>
+          <t>Private</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
splitting of part 4 and other small things
</commit_message>
<xml_diff>
--- a/out/diabetes_join.xlsx
+++ b/out/diabetes_join.xlsx
@@ -351,7 +351,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:K491"/>
+  <dimension ref="A1:K532"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -450,16 +450,6 @@
       <c r="I2">
         <v>9.800000000000001</v>
       </c>
-      <c r="J2" t="inlineStr">
-        <is>
-          <t>Yes</t>
-        </is>
-      </c>
-      <c r="K2" t="inlineStr">
-        <is>
-          <t>Self-employed</t>
-        </is>
-      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -497,16 +487,6 @@
       <c r="I3">
         <v>9.5</v>
       </c>
-      <c r="J3" t="inlineStr">
-        <is>
-          <t>No</t>
-        </is>
-      </c>
-      <c r="K3" t="inlineStr">
-        <is>
-          <t>Public</t>
-        </is>
-      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -544,16 +524,6 @@
       <c r="I4">
         <v>9.4</v>
       </c>
-      <c r="J4" t="inlineStr">
-        <is>
-          <t>Yes</t>
-        </is>
-      </c>
-      <c r="K4" t="inlineStr">
-        <is>
-          <t>Self-employed</t>
-        </is>
-      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -591,16 +561,6 @@
       <c r="I5">
         <v>9</v>
       </c>
-      <c r="J5" t="inlineStr">
-        <is>
-          <t>Yes</t>
-        </is>
-      </c>
-      <c r="K5" t="inlineStr">
-        <is>
-          <t>Private</t>
-        </is>
-      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -638,16 +598,6 @@
       <c r="I6">
         <v>9.300000000000001</v>
       </c>
-      <c r="J6" t="inlineStr">
-        <is>
-          <t>Yes</t>
-        </is>
-      </c>
-      <c r="K6" t="inlineStr">
-        <is>
-          <t>Private</t>
-        </is>
-      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -685,16 +635,6 @@
       <c r="I7">
         <v>9.6</v>
       </c>
-      <c r="J7" t="inlineStr">
-        <is>
-          <t>Yes</t>
-        </is>
-      </c>
-      <c r="K7" t="inlineStr">
-        <is>
-          <t>Private</t>
-        </is>
-      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -732,16 +672,6 @@
       <c r="I8">
         <v>9.1</v>
       </c>
-      <c r="J8" t="inlineStr">
-        <is>
-          <t>Yes</t>
-        </is>
-      </c>
-      <c r="K8" t="inlineStr">
-        <is>
-          <t>Self-employed</t>
-        </is>
-      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -779,16 +709,6 @@
       <c r="I9">
         <v>9.300000000000001</v>
       </c>
-      <c r="J9" t="inlineStr">
-        <is>
-          <t>No</t>
-        </is>
-      </c>
-      <c r="K9" t="inlineStr">
-        <is>
-          <t>Private</t>
-        </is>
-      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -826,16 +746,6 @@
       <c r="I10">
         <v>9.1</v>
       </c>
-      <c r="J10" t="inlineStr">
-        <is>
-          <t>Yes</t>
-        </is>
-      </c>
-      <c r="K10" t="inlineStr">
-        <is>
-          <t>Private</t>
-        </is>
-      </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -873,16 +783,6 @@
       <c r="I11">
         <v>9.5</v>
       </c>
-      <c r="J11" t="inlineStr">
-        <is>
-          <t>Yes</t>
-        </is>
-      </c>
-      <c r="K11" t="inlineStr">
-        <is>
-          <t>Private</t>
-        </is>
-      </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -920,16 +820,6 @@
       <c r="I12">
         <v>9.1</v>
       </c>
-      <c r="J12" t="inlineStr">
-        <is>
-          <t>No</t>
-        </is>
-      </c>
-      <c r="K12" t="inlineStr">
-        <is>
-          <t>Private</t>
-        </is>
-      </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -967,16 +857,6 @@
       <c r="I13">
         <v>9.6</v>
       </c>
-      <c r="J13" t="inlineStr">
-        <is>
-          <t>No</t>
-        </is>
-      </c>
-      <c r="K13" t="inlineStr">
-        <is>
-          <t>Public</t>
-        </is>
-      </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -1014,16 +894,6 @@
       <c r="I14">
         <v>9.5</v>
       </c>
-      <c r="J14" t="inlineStr">
-        <is>
-          <t>Yes</t>
-        </is>
-      </c>
-      <c r="K14" t="inlineStr">
-        <is>
-          <t>Private</t>
-        </is>
-      </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -1061,16 +931,6 @@
       <c r="I15">
         <v>9.6</v>
       </c>
-      <c r="J15" t="inlineStr">
-        <is>
-          <t>No</t>
-        </is>
-      </c>
-      <c r="K15" t="inlineStr">
-        <is>
-          <t>Private</t>
-        </is>
-      </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -1108,16 +968,6 @@
       <c r="I16">
         <v>9.6</v>
       </c>
-      <c r="J16" t="inlineStr">
-        <is>
-          <t>No</t>
-        </is>
-      </c>
-      <c r="K16" t="inlineStr">
-        <is>
-          <t>Public</t>
-        </is>
-      </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
@@ -1155,16 +1005,6 @@
       <c r="I17">
         <v>9.699999999999999</v>
       </c>
-      <c r="J17" t="inlineStr">
-        <is>
-          <t>No</t>
-        </is>
-      </c>
-      <c r="K17" t="inlineStr">
-        <is>
-          <t>Public</t>
-        </is>
-      </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
@@ -23433,6 +23273,703 @@
         </is>
       </c>
       <c r="K491" t="inlineStr">
+        <is>
+          <t>Self-employed</t>
+        </is>
+      </c>
+    </row>
+    <row r="492">
+      <c r="A492" t="inlineStr">
+        <is>
+          <t>27832</t>
+        </is>
+      </c>
+      <c r="J492" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="K492" t="inlineStr">
+        <is>
+          <t>Private</t>
+        </is>
+      </c>
+    </row>
+    <row r="493">
+      <c r="A493" t="inlineStr">
+        <is>
+          <t>58978</t>
+        </is>
+      </c>
+      <c r="J493" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="K493" t="inlineStr">
+        <is>
+          <t>Private</t>
+        </is>
+      </c>
+    </row>
+    <row r="494">
+      <c r="A494" t="inlineStr">
+        <is>
+          <t>34376</t>
+        </is>
+      </c>
+      <c r="J494" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="K494" t="inlineStr">
+        <is>
+          <t>Public</t>
+        </is>
+      </c>
+    </row>
+    <row r="495">
+      <c r="A495" t="inlineStr">
+        <is>
+          <t>67432</t>
+        </is>
+      </c>
+      <c r="J495" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="K495" t="inlineStr">
+        <is>
+          <t>Private</t>
+        </is>
+      </c>
+    </row>
+    <row r="496">
+      <c r="A496" t="inlineStr">
+        <is>
+          <t>56681</t>
+        </is>
+      </c>
+      <c r="J496" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="K496" t="inlineStr">
+        <is>
+          <t>Private</t>
+        </is>
+      </c>
+    </row>
+    <row r="497">
+      <c r="A497" t="inlineStr">
+        <is>
+          <t>71038</t>
+        </is>
+      </c>
+      <c r="J497" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="K497" t="inlineStr">
+        <is>
+          <t>Public</t>
+        </is>
+      </c>
+    </row>
+    <row r="498">
+      <c r="A498" t="inlineStr">
+        <is>
+          <t>58631</t>
+        </is>
+      </c>
+      <c r="J498" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="K498" t="inlineStr">
+        <is>
+          <t>Self-employed</t>
+        </is>
+      </c>
+    </row>
+    <row r="499">
+      <c r="A499" t="inlineStr">
+        <is>
+          <t>42072</t>
+        </is>
+      </c>
+      <c r="J499" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="K499" t="inlineStr">
+        <is>
+          <t>Self-employed</t>
+        </is>
+      </c>
+    </row>
+    <row r="500">
+      <c r="A500" t="inlineStr">
+        <is>
+          <t>66400</t>
+        </is>
+      </c>
+      <c r="J500" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="K500" t="inlineStr">
+        <is>
+          <t>Retired</t>
+        </is>
+      </c>
+    </row>
+    <row r="501">
+      <c r="A501" t="inlineStr">
+        <is>
+          <t>11974</t>
+        </is>
+      </c>
+      <c r="J501" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="K501" t="inlineStr">
+        <is>
+          <t>Public</t>
+        </is>
+      </c>
+    </row>
+    <row r="502">
+      <c r="A502" t="inlineStr">
+        <is>
+          <t>67177</t>
+        </is>
+      </c>
+      <c r="J502" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="K502" t="inlineStr">
+        <is>
+          <t>Private</t>
+        </is>
+      </c>
+    </row>
+    <row r="503">
+      <c r="A503" t="inlineStr">
+        <is>
+          <t>25774</t>
+        </is>
+      </c>
+      <c r="J503" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="K503" t="inlineStr">
+        <is>
+          <t>Private</t>
+        </is>
+      </c>
+    </row>
+    <row r="504">
+      <c r="A504" t="inlineStr">
+        <is>
+          <t>46785</t>
+        </is>
+      </c>
+      <c r="J504" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="K504" t="inlineStr">
+        <is>
+          <t>Private</t>
+        </is>
+      </c>
+    </row>
+    <row r="505">
+      <c r="A505" t="inlineStr">
+        <is>
+          <t>54375</t>
+        </is>
+      </c>
+      <c r="J505" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="K505" t="inlineStr">
+        <is>
+          <t>Public</t>
+        </is>
+      </c>
+    </row>
+    <row r="506">
+      <c r="A506" t="inlineStr">
+        <is>
+          <t>2182</t>
+        </is>
+      </c>
+      <c r="J506" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="K506" t="inlineStr">
+        <is>
+          <t>Public</t>
+        </is>
+      </c>
+    </row>
+    <row r="507">
+      <c r="A507" t="inlineStr">
+        <is>
+          <t>26325</t>
+        </is>
+      </c>
+      <c r="J507" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="K507" t="inlineStr">
+        <is>
+          <t>Private</t>
+        </is>
+      </c>
+    </row>
+    <row r="508">
+      <c r="A508" t="inlineStr">
+        <is>
+          <t>48796</t>
+        </is>
+      </c>
+      <c r="J508" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="K508" t="inlineStr">
+        <is>
+          <t>Private</t>
+        </is>
+      </c>
+    </row>
+    <row r="509">
+      <c r="A509" t="inlineStr">
+        <is>
+          <t>56546</t>
+        </is>
+      </c>
+      <c r="J509" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="K509" t="inlineStr">
+        <is>
+          <t>Private</t>
+        </is>
+      </c>
+    </row>
+    <row r="510">
+      <c r="A510" t="inlineStr">
+        <is>
+          <t>28645</t>
+        </is>
+      </c>
+      <c r="J510" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="K510" t="inlineStr">
+        <is>
+          <t>Private</t>
+        </is>
+      </c>
+    </row>
+    <row r="511">
+      <c r="A511" t="inlineStr">
+        <is>
+          <t>54385</t>
+        </is>
+      </c>
+      <c r="J511" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="K511" t="inlineStr">
+        <is>
+          <t>Self-employed</t>
+        </is>
+      </c>
+    </row>
+    <row r="512">
+      <c r="A512" t="inlineStr">
+        <is>
+          <t>11091</t>
+        </is>
+      </c>
+      <c r="J512" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="K512" t="inlineStr">
+        <is>
+          <t>Private</t>
+        </is>
+      </c>
+    </row>
+    <row r="513">
+      <c r="A513" t="inlineStr">
+        <is>
+          <t>17718</t>
+        </is>
+      </c>
+      <c r="J513" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="K513" t="inlineStr">
+        <is>
+          <t>Retired</t>
+        </is>
+      </c>
+    </row>
+    <row r="514">
+      <c r="A514" t="inlineStr">
+        <is>
+          <t>30468</t>
+        </is>
+      </c>
+      <c r="J514" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="K514" t="inlineStr">
+        <is>
+          <t>Public</t>
+        </is>
+      </c>
+    </row>
+    <row r="515">
+      <c r="A515" t="inlineStr">
+        <is>
+          <t>4651</t>
+        </is>
+      </c>
+      <c r="J515" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="K515" t="inlineStr">
+        <is>
+          <t>Private</t>
+        </is>
+      </c>
+    </row>
+    <row r="516">
+      <c r="A516" t="inlineStr">
+        <is>
+          <t>36236</t>
+        </is>
+      </c>
+      <c r="J516" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="K516" t="inlineStr">
+        <is>
+          <t>Private</t>
+        </is>
+      </c>
+    </row>
+    <row r="517">
+      <c r="A517" t="inlineStr">
+        <is>
+          <t>31179</t>
+        </is>
+      </c>
+      <c r="J517" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="K517" t="inlineStr">
+        <is>
+          <t>Private</t>
+        </is>
+      </c>
+    </row>
+    <row r="518">
+      <c r="A518" t="inlineStr">
+        <is>
+          <t>68627</t>
+        </is>
+      </c>
+      <c r="J518" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="K518" t="inlineStr">
+        <is>
+          <t>Private</t>
+        </is>
+      </c>
+    </row>
+    <row r="519">
+      <c r="A519" t="inlineStr">
+        <is>
+          <t>18587</t>
+        </is>
+      </c>
+      <c r="J519" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="K519" t="inlineStr">
+        <is>
+          <t>Self-employed</t>
+        </is>
+      </c>
+    </row>
+    <row r="520">
+      <c r="A520" t="inlineStr">
+        <is>
+          <t>50931</t>
+        </is>
+      </c>
+      <c r="J520" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="K520" t="inlineStr">
+        <is>
+          <t>Public</t>
+        </is>
+      </c>
+    </row>
+    <row r="521">
+      <c r="A521" t="inlineStr">
+        <is>
+          <t>32503</t>
+        </is>
+      </c>
+      <c r="J521" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="K521" t="inlineStr">
+        <is>
+          <t>Self-employed</t>
+        </is>
+      </c>
+    </row>
+    <row r="522">
+      <c r="A522" t="inlineStr">
+        <is>
+          <t>43054</t>
+        </is>
+      </c>
+      <c r="J522" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="K522" t="inlineStr">
+        <is>
+          <t>Private</t>
+        </is>
+      </c>
+    </row>
+    <row r="523">
+      <c r="A523" t="inlineStr">
+        <is>
+          <t>38165</t>
+        </is>
+      </c>
+      <c r="J523" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="K523" t="inlineStr">
+        <is>
+          <t>Private</t>
+        </is>
+      </c>
+    </row>
+    <row r="524">
+      <c r="A524" t="inlineStr">
+        <is>
+          <t>6118</t>
+        </is>
+      </c>
+      <c r="J524" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="K524" t="inlineStr">
+        <is>
+          <t>Private</t>
+        </is>
+      </c>
+    </row>
+    <row r="525">
+      <c r="A525" t="inlineStr">
+        <is>
+          <t>16371</t>
+        </is>
+      </c>
+      <c r="J525" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="K525" t="inlineStr">
+        <is>
+          <t>Self-employed</t>
+        </is>
+      </c>
+    </row>
+    <row r="526">
+      <c r="A526" t="inlineStr">
+        <is>
+          <t>69551</t>
+        </is>
+      </c>
+      <c r="J526" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="K526" t="inlineStr">
+        <is>
+          <t>Public</t>
+        </is>
+      </c>
+    </row>
+    <row r="527">
+      <c r="A527" t="inlineStr">
+        <is>
+          <t>64908</t>
+        </is>
+      </c>
+      <c r="J527" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="K527" t="inlineStr">
+        <is>
+          <t>Private</t>
+        </is>
+      </c>
+    </row>
+    <row r="528">
+      <c r="A528" t="inlineStr">
+        <is>
+          <t>30456</t>
+        </is>
+      </c>
+      <c r="J528" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="K528" t="inlineStr">
+        <is>
+          <t>Private</t>
+        </is>
+      </c>
+    </row>
+    <row r="529">
+      <c r="A529" t="inlineStr">
+        <is>
+          <t>39373</t>
+        </is>
+      </c>
+      <c r="J529" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="K529" t="inlineStr">
+        <is>
+          <t>Self-employed</t>
+        </is>
+      </c>
+    </row>
+    <row r="530">
+      <c r="A530" t="inlineStr">
+        <is>
+          <t>70822</t>
+        </is>
+      </c>
+      <c r="J530" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="K530" t="inlineStr">
+        <is>
+          <t>Public</t>
+        </is>
+      </c>
+    </row>
+    <row r="531">
+      <c r="A531" t="inlineStr">
+        <is>
+          <t>21408</t>
+        </is>
+      </c>
+      <c r="J531" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="K531" t="inlineStr">
+        <is>
+          <t>Self-employed</t>
+        </is>
+      </c>
+    </row>
+    <row r="532">
+      <c r="A532" t="inlineStr">
+        <is>
+          <t>25226</t>
+        </is>
+      </c>
+      <c r="J532" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="K532" t="inlineStr">
         <is>
           <t>Self-employed</t>
         </is>

</xml_diff>

<commit_message>
Exercises and Solutions 5A and 5B done
</commit_message>
<xml_diff>
--- a/out/diabetes_join.xlsx
+++ b/out/diabetes_join.xlsx
@@ -23281,41 +23281,41 @@
     <row r="492">
       <c r="A492" t="inlineStr">
         <is>
-          <t>27832</t>
+          <t>34376</t>
         </is>
       </c>
       <c r="J492" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="K492" t="inlineStr">
         <is>
-          <t>Private</t>
+          <t>Public</t>
         </is>
       </c>
     </row>
     <row r="493">
       <c r="A493" t="inlineStr">
         <is>
-          <t>58978</t>
+          <t>70822</t>
         </is>
       </c>
       <c r="J493" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="K493" t="inlineStr">
         <is>
-          <t>Private</t>
+          <t>Public</t>
         </is>
       </c>
     </row>
     <row r="494">
       <c r="A494" t="inlineStr">
         <is>
-          <t>34376</t>
+          <t>36236</t>
         </is>
       </c>
       <c r="J494" t="inlineStr">
@@ -23325,14 +23325,14 @@
       </c>
       <c r="K494" t="inlineStr">
         <is>
-          <t>Public</t>
+          <t>Private</t>
         </is>
       </c>
     </row>
     <row r="495">
       <c r="A495" t="inlineStr">
         <is>
-          <t>67432</t>
+          <t>25226</t>
         </is>
       </c>
       <c r="J495" t="inlineStr">
@@ -23342,31 +23342,31 @@
       </c>
       <c r="K495" t="inlineStr">
         <is>
-          <t>Private</t>
+          <t>Self-employed</t>
         </is>
       </c>
     </row>
     <row r="496">
       <c r="A496" t="inlineStr">
         <is>
-          <t>56681</t>
+          <t>2182</t>
         </is>
       </c>
       <c r="J496" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="K496" t="inlineStr">
         <is>
-          <t>Private</t>
+          <t>Public</t>
         </is>
       </c>
     </row>
     <row r="497">
       <c r="A497" t="inlineStr">
         <is>
-          <t>71038</t>
+          <t>67177</t>
         </is>
       </c>
       <c r="J497" t="inlineStr">
@@ -23376,14 +23376,14 @@
       </c>
       <c r="K497" t="inlineStr">
         <is>
-          <t>Public</t>
+          <t>Private</t>
         </is>
       </c>
     </row>
     <row r="498">
       <c r="A498" t="inlineStr">
         <is>
-          <t>58631</t>
+          <t>39373</t>
         </is>
       </c>
       <c r="J498" t="inlineStr">
@@ -23400,24 +23400,24 @@
     <row r="499">
       <c r="A499" t="inlineStr">
         <is>
-          <t>42072</t>
+          <t>11974</t>
         </is>
       </c>
       <c r="J499" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="K499" t="inlineStr">
         <is>
-          <t>Self-employed</t>
+          <t>Public</t>
         </is>
       </c>
     </row>
     <row r="500">
       <c r="A500" t="inlineStr">
         <is>
-          <t>66400</t>
+          <t>28645</t>
         </is>
       </c>
       <c r="J500" t="inlineStr">
@@ -23427,36 +23427,36 @@
       </c>
       <c r="K500" t="inlineStr">
         <is>
-          <t>Retired</t>
+          <t>Private</t>
         </is>
       </c>
     </row>
     <row r="501">
       <c r="A501" t="inlineStr">
         <is>
-          <t>11974</t>
+          <t>56681</t>
         </is>
       </c>
       <c r="J501" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="K501" t="inlineStr">
         <is>
-          <t>Public</t>
+          <t>Private</t>
         </is>
       </c>
     </row>
     <row r="502">
       <c r="A502" t="inlineStr">
         <is>
-          <t>67177</t>
+          <t>56546</t>
         </is>
       </c>
       <c r="J502" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="K502" t="inlineStr">
@@ -23468,7 +23468,7 @@
     <row r="503">
       <c r="A503" t="inlineStr">
         <is>
-          <t>25774</t>
+          <t>21408</t>
         </is>
       </c>
       <c r="J503" t="inlineStr">
@@ -23478,14 +23478,14 @@
       </c>
       <c r="K503" t="inlineStr">
         <is>
-          <t>Private</t>
+          <t>Self-employed</t>
         </is>
       </c>
     </row>
     <row r="504">
       <c r="A504" t="inlineStr">
         <is>
-          <t>46785</t>
+          <t>66400</t>
         </is>
       </c>
       <c r="J504" t="inlineStr">
@@ -23495,19 +23495,19 @@
       </c>
       <c r="K504" t="inlineStr">
         <is>
-          <t>Private</t>
+          <t>Retired</t>
         </is>
       </c>
     </row>
     <row r="505">
       <c r="A505" t="inlineStr">
         <is>
-          <t>54375</t>
+          <t>71038</t>
         </is>
       </c>
       <c r="J505" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="K505" t="inlineStr">
@@ -23519,41 +23519,41 @@
     <row r="506">
       <c r="A506" t="inlineStr">
         <is>
-          <t>2182</t>
+          <t>46785</t>
         </is>
       </c>
       <c r="J506" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="K506" t="inlineStr">
         <is>
-          <t>Public</t>
+          <t>Private</t>
         </is>
       </c>
     </row>
     <row r="507">
       <c r="A507" t="inlineStr">
         <is>
-          <t>26325</t>
+          <t>50931</t>
         </is>
       </c>
       <c r="J507" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="K507" t="inlineStr">
         <is>
-          <t>Private</t>
+          <t>Public</t>
         </is>
       </c>
     </row>
     <row r="508">
       <c r="A508" t="inlineStr">
         <is>
-          <t>48796</t>
+          <t>58978</t>
         </is>
       </c>
       <c r="J508" t="inlineStr">
@@ -23570,7 +23570,7 @@
     <row r="509">
       <c r="A509" t="inlineStr">
         <is>
-          <t>56546</t>
+          <t>11091</t>
         </is>
       </c>
       <c r="J509" t="inlineStr">
@@ -23587,58 +23587,58 @@
     <row r="510">
       <c r="A510" t="inlineStr">
         <is>
-          <t>28645</t>
+          <t>32503</t>
         </is>
       </c>
       <c r="J510" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="K510" t="inlineStr">
         <is>
-          <t>Private</t>
+          <t>Self-employed</t>
         </is>
       </c>
     </row>
     <row r="511">
       <c r="A511" t="inlineStr">
         <is>
-          <t>54385</t>
+          <t>4651</t>
         </is>
       </c>
       <c r="J511" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="K511" t="inlineStr">
         <is>
-          <t>Self-employed</t>
+          <t>Private</t>
         </is>
       </c>
     </row>
     <row r="512">
       <c r="A512" t="inlineStr">
         <is>
-          <t>11091</t>
+          <t>54385</t>
         </is>
       </c>
       <c r="J512" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="K512" t="inlineStr">
         <is>
-          <t>Private</t>
+          <t>Self-employed</t>
         </is>
       </c>
     </row>
     <row r="513">
       <c r="A513" t="inlineStr">
         <is>
-          <t>17718</t>
+          <t>25774</t>
         </is>
       </c>
       <c r="J513" t="inlineStr">
@@ -23648,31 +23648,31 @@
       </c>
       <c r="K513" t="inlineStr">
         <is>
-          <t>Retired</t>
+          <t>Private</t>
         </is>
       </c>
     </row>
     <row r="514">
       <c r="A514" t="inlineStr">
         <is>
-          <t>30468</t>
+          <t>17718</t>
         </is>
       </c>
       <c r="J514" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="K514" t="inlineStr">
         <is>
-          <t>Public</t>
+          <t>Retired</t>
         </is>
       </c>
     </row>
     <row r="515">
       <c r="A515" t="inlineStr">
         <is>
-          <t>4651</t>
+          <t>43054</t>
         </is>
       </c>
       <c r="J515" t="inlineStr">
@@ -23689,24 +23689,24 @@
     <row r="516">
       <c r="A516" t="inlineStr">
         <is>
-          <t>36236</t>
+          <t>42072</t>
         </is>
       </c>
       <c r="J516" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="K516" t="inlineStr">
         <is>
-          <t>Private</t>
+          <t>Self-employed</t>
         </is>
       </c>
     </row>
     <row r="517">
       <c r="A517" t="inlineStr">
         <is>
-          <t>31179</t>
+          <t>64908</t>
         </is>
       </c>
       <c r="J517" t="inlineStr">
@@ -23723,7 +23723,7 @@
     <row r="518">
       <c r="A518" t="inlineStr">
         <is>
-          <t>68627</t>
+          <t>67432</t>
         </is>
       </c>
       <c r="J518" t="inlineStr">
@@ -23757,7 +23757,7 @@
     <row r="520">
       <c r="A520" t="inlineStr">
         <is>
-          <t>50931</t>
+          <t>38165</t>
         </is>
       </c>
       <c r="J520" t="inlineStr">
@@ -23767,31 +23767,31 @@
       </c>
       <c r="K520" t="inlineStr">
         <is>
-          <t>Public</t>
+          <t>Private</t>
         </is>
       </c>
     </row>
     <row r="521">
       <c r="A521" t="inlineStr">
         <is>
-          <t>32503</t>
+          <t>54375</t>
         </is>
       </c>
       <c r="J521" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="K521" t="inlineStr">
         <is>
-          <t>Self-employed</t>
+          <t>Public</t>
         </is>
       </c>
     </row>
     <row r="522">
       <c r="A522" t="inlineStr">
         <is>
-          <t>43054</t>
+          <t>58631</t>
         </is>
       </c>
       <c r="J522" t="inlineStr">
@@ -23801,19 +23801,19 @@
       </c>
       <c r="K522" t="inlineStr">
         <is>
-          <t>Private</t>
+          <t>Self-employed</t>
         </is>
       </c>
     </row>
     <row r="523">
       <c r="A523" t="inlineStr">
         <is>
-          <t>38165</t>
+          <t>26325</t>
         </is>
       </c>
       <c r="J523" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="K523" t="inlineStr">
@@ -23825,12 +23825,12 @@
     <row r="524">
       <c r="A524" t="inlineStr">
         <is>
-          <t>6118</t>
+          <t>27832</t>
         </is>
       </c>
       <c r="J524" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="K524" t="inlineStr">
@@ -23842,17 +23842,17 @@
     <row r="525">
       <c r="A525" t="inlineStr">
         <is>
-          <t>16371</t>
+          <t>6118</t>
         </is>
       </c>
       <c r="J525" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="K525" t="inlineStr">
         <is>
-          <t>Self-employed</t>
+          <t>Private</t>
         </is>
       </c>
     </row>
@@ -23876,7 +23876,7 @@
     <row r="527">
       <c r="A527" t="inlineStr">
         <is>
-          <t>64908</t>
+          <t>16371</t>
         </is>
       </c>
       <c r="J527" t="inlineStr">
@@ -23886,19 +23886,19 @@
       </c>
       <c r="K527" t="inlineStr">
         <is>
-          <t>Private</t>
+          <t>Self-employed</t>
         </is>
       </c>
     </row>
     <row r="528">
       <c r="A528" t="inlineStr">
         <is>
-          <t>30456</t>
+          <t>31179</t>
         </is>
       </c>
       <c r="J528" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="K528" t="inlineStr">
@@ -23910,58 +23910,58 @@
     <row r="529">
       <c r="A529" t="inlineStr">
         <is>
-          <t>39373</t>
+          <t>30456</t>
         </is>
       </c>
       <c r="J529" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="K529" t="inlineStr">
         <is>
-          <t>Self-employed</t>
+          <t>Private</t>
         </is>
       </c>
     </row>
     <row r="530">
       <c r="A530" t="inlineStr">
         <is>
-          <t>70822</t>
+          <t>68627</t>
         </is>
       </c>
       <c r="J530" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="K530" t="inlineStr">
         <is>
-          <t>Public</t>
+          <t>Private</t>
         </is>
       </c>
     </row>
     <row r="531">
       <c r="A531" t="inlineStr">
         <is>
-          <t>21408</t>
+          <t>30468</t>
         </is>
       </c>
       <c r="J531" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="K531" t="inlineStr">
         <is>
-          <t>Self-employed</t>
+          <t>Public</t>
         </is>
       </c>
     </row>
     <row r="532">
       <c r="A532" t="inlineStr">
         <is>
-          <t>25226</t>
+          <t>48796</t>
         </is>
       </c>
       <c r="J532" t="inlineStr">
@@ -23971,7 +23971,7 @@
       </c>
       <c r="K532" t="inlineStr">
         <is>
-          <t>Self-employed</t>
+          <t>Private</t>
         </is>
       </c>
     </row>

</xml_diff>